<commit_message>
Removing merge cells to prevent issues on generating xlsx
</commit_message>
<xml_diff>
--- a/server/templates/analysisRequest/analysisRequest.xlsx
+++ b/server/templates/analysisRequest/analysisRequest.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="69">
   <si>
     <t>Demande d'Analyse Informatisée</t>
   </si>
@@ -46,27 +46,27 @@
     <t>Heure de prélèvement</t>
   </si>
   <si>
+    <t>{d.sampledAtDate}</t>
+  </si>
+  <si>
+    <t>{d.sampledAtTime}</t>
+  </si>
+  <si>
+    <t>Numéro de prélèvement</t>
+  </si>
+  <si>
+    <t>{d.reference}</t>
+  </si>
+  <si>
     <t>Contexte du prélèvement</t>
   </si>
   <si>
-    <t>{d.sampledAtDate}</t>
-  </si>
-  <si>
-    <t>{d.sampledAtTime}</t>
+    <t>Cadre juridique</t>
   </si>
   <si>
     <t>{d.context}</t>
   </si>
   <si>
-    <t>Numéro de prélèvement</t>
-  </si>
-  <si>
-    <t>Cadre juridique</t>
-  </si>
-  <si>
-    <t>{d.reference}</t>
-  </si>
-  <si>
     <t>{d.legalContext}</t>
   </si>
   <si>
@@ -169,31 +169,23 @@
     <t>{d.monoSubstances[i].code}</t>
   </si>
   <si>
-    <t xml:space="preserve">{d.monoSubstances[i+1].label}
+    <t xml:space="preserve">{d.monoSubstances[i+1]}
 </t>
   </si>
   <si>
-    <t xml:space="preserve">{d.monoSubstances[i+1].code}
+    <t>Analyses multi-résidus dont :</t>
+  </si>
+  <si>
+    <t>{d.multiSubstances[i].label}</t>
+  </si>
+  <si>
+    <t>{d.multiSubstances[i].code}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{d.multiSubstances[i+1]}
 </t>
   </si>
   <si>
-    <t>Analyses multi-résidus dont :</t>
-  </si>
-  <si>
-    <t>{d.multiSubstances[i].label}</t>
-  </si>
-  <si>
-    <t>{d.multiSubstances[i].code}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{d.multiSubstances[i+1].label}
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{d.multiSubstances[i+1].code}
-</t>
-  </si>
-  <si>
     <t>{d.notesOnMatrix}</t>
   </si>
   <si>
@@ -206,16 +198,16 @@
     <t>Unité de mesure</t>
   </si>
   <si>
+    <t>{d.quantity}</t>
+  </si>
+  <si>
+    <t>{d.quantityUnit}</t>
+  </si>
+  <si>
     <t>Numéro de scellé</t>
   </si>
   <si>
     <t>Directive 2002/63</t>
-  </si>
-  <si>
-    <t>{d.quantity}</t>
-  </si>
-  <si>
-    <t>{d.quantityUnit}</t>
   </si>
   <si>
     <t>{d.sealId}</t>
@@ -274,7 +266,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -302,21 +294,6 @@
         <color indexed="8"/>
       </left>
       <right style="thick">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="8"/>
-      </left>
-      <right style="medium">
         <color indexed="8"/>
       </right>
       <top style="medium">
@@ -359,12 +336,27 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
       </left>
       <right>
         <color indexed="8"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="8"/>
       </top>
       <bottom style="thin">
@@ -377,7 +369,7 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
@@ -392,13 +384,28 @@
         <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="8"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
       </bottom>
       <diagonal/>
     </border>
@@ -407,81 +414,6 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left>
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right>
         <color indexed="8"/>
       </right>
       <top style="thin">
@@ -498,7 +430,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -509,75 +441,60 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1711,14 +1628,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:B47"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="4" width="25" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="1" max="2" width="50" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="61" customHeight="1">
@@ -1726,470 +1643,336 @@
         <v>0</v>
       </c>
       <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
     </row>
     <row r="2" ht="14.55" customHeight="1">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="5"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="8">
+      <c r="A3" t="s" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" t="s" s="8">
+      <c r="B3" t="s" s="6">
         <v>2</v>
       </c>
-      <c r="D3" s="9"/>
     </row>
     <row r="4" ht="42" customHeight="1">
-      <c r="A4" t="s" s="10">
+      <c r="A4" t="s" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" t="s" s="10">
+      <c r="B4" t="s" s="7">
         <v>4</v>
       </c>
-      <c r="D4" s="11"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="14"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" t="s" s="8">
+      <c r="A6" t="s" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" t="s" s="8">
+      <c r="B6" t="s" s="6">
         <v>6</v>
       </c>
-      <c r="D6" s="9"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" t="s" s="10">
+      <c r="A7" t="s" s="7">
         <v>7</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" t="s" s="10">
+      <c r="B7" t="s" s="7">
         <v>8</v>
       </c>
-      <c r="D7" s="11"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" t="s" s="8">
+      <c r="A9" t="s" s="6">
         <v>9</v>
       </c>
-      <c r="B9" t="s" s="8">
+      <c r="B9" t="s" s="6">
         <v>10</v>
       </c>
-      <c r="C9" t="s" s="8">
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" t="s" s="9">
         <v>11</v>
       </c>
-      <c r="D9" s="9"/>
-    </row>
-    <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" t="s" s="15">
+      <c r="B10" t="s" s="10">
         <v>12</v>
       </c>
-      <c r="B10" t="s" s="15">
+    </row>
+    <row r="11" ht="13.55" customHeight="1">
+      <c r="A11" t="s" s="11">
         <v>13</v>
       </c>
-      <c r="C10" t="s" s="15">
+      <c r="B11" s="12"/>
+    </row>
+    <row r="12" ht="13.55" customHeight="1">
+      <c r="A12" t="s" s="13">
         <v>14</v>
       </c>
-      <c r="D10" s="16"/>
-    </row>
-    <row r="11" ht="13.55" customHeight="1">
-      <c r="A11" t="s" s="8">
+      <c r="B12" s="14"/>
+    </row>
+    <row r="13" ht="13.55" customHeight="1">
+      <c r="A13" t="s" s="6">
         <v>15</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" t="s" s="8">
+      <c r="B13" t="s" s="6">
         <v>16</v>
       </c>
-      <c r="D11" s="9"/>
-    </row>
-    <row r="12" ht="13.55" customHeight="1">
-      <c r="A12" t="s" s="15">
+    </row>
+    <row r="14" ht="13.55" customHeight="1">
+      <c r="A14" t="s" s="9">
         <v>17</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" t="s" s="15">
+      <c r="B14" t="s" s="10">
         <v>18</v>
       </c>
-      <c r="D12" s="16"/>
-    </row>
-    <row r="13" ht="13.55" customHeight="1">
-      <c r="A13" t="s" s="8">
+    </row>
+    <row r="15" ht="13.55" customHeight="1">
+      <c r="A15" t="s" s="6">
         <v>19</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" t="s" s="8">
+      <c r="B15" t="s" s="6">
         <v>20</v>
       </c>
-      <c r="D13" s="9"/>
-    </row>
-    <row r="14" ht="13.55" customHeight="1">
-      <c r="A14" t="s" s="15">
+    </row>
+    <row r="16" ht="13.55" customHeight="1">
+      <c r="A16" t="s" s="9">
         <v>21</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" t="s" s="15">
+      <c r="B16" t="s" s="10">
         <v>22</v>
       </c>
-      <c r="D14" s="16"/>
-    </row>
-    <row r="15" ht="13.55" customHeight="1">
-      <c r="A15" t="s" s="8">
+    </row>
+    <row r="17" ht="13.55" customHeight="1">
+      <c r="A17" t="s" s="6">
         <v>23</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" t="s" s="8">
+      <c r="B17" t="s" s="6">
         <v>24</v>
       </c>
-      <c r="D15" s="9"/>
-    </row>
-    <row r="16" ht="13.55" customHeight="1">
-      <c r="A16" t="s" s="15">
+    </row>
+    <row r="18" ht="13.55" customHeight="1">
+      <c r="A18" t="s" s="9">
         <v>25</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" t="s" s="15">
+      <c r="B18" t="s" s="10">
         <v>26</v>
       </c>
-      <c r="D16" s="16"/>
-    </row>
-    <row r="17" ht="13.55" customHeight="1">
-      <c r="A17" t="s" s="8">
+    </row>
+    <row r="19" ht="13.55" customHeight="1">
+      <c r="A19" t="s" s="6">
         <v>2</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" t="s" s="8">
+      <c r="B19" t="s" s="6">
         <v>27</v>
       </c>
-      <c r="D17" s="9"/>
-    </row>
-    <row r="18" ht="28" customHeight="1">
-      <c r="A18" t="s" s="15">
+    </row>
+    <row r="20" ht="28" customHeight="1">
+      <c r="A20" t="s" s="9">
         <v>28</v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" t="s" s="15">
+      <c r="B20" t="s" s="10">
         <v>29</v>
       </c>
-      <c r="D18" s="16"/>
-    </row>
-    <row r="19" ht="13.55" customHeight="1">
-      <c r="A19" t="s" s="8">
+    </row>
+    <row r="21" ht="13.55" customHeight="1">
+      <c r="A21" t="s" s="11">
         <v>30</v>
       </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-    </row>
-    <row r="20" ht="13.55" customHeight="1">
-      <c r="A20" t="s" s="15">
+      <c r="B21" s="12"/>
+    </row>
+    <row r="22" ht="13.55" customHeight="1">
+      <c r="A22" t="s" s="13">
         <v>31</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-    </row>
-    <row r="21" ht="13.55" customHeight="1">
-      <c r="A21" s="18"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="19"/>
-    </row>
-    <row r="22" ht="13.55" customHeight="1">
-      <c r="A22" t="s" s="8">
+      <c r="B22" s="15"/>
+    </row>
+    <row r="23" ht="13.55" customHeight="1">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+    </row>
+    <row r="24" ht="13.55" customHeight="1">
+      <c r="A24" t="s" s="6">
         <v>32</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" t="s" s="8">
+      <c r="B24" t="s" s="6">
         <v>33</v>
       </c>
-      <c r="D22" s="9"/>
-    </row>
-    <row r="23" ht="13.55" customHeight="1">
-      <c r="A23" t="s" s="15">
+    </row>
+    <row r="25" ht="13.55" customHeight="1">
+      <c r="A25" t="s" s="7">
         <v>34</v>
       </c>
-      <c r="B23" s="16"/>
-      <c r="C23" t="s" s="15">
+      <c r="B25" t="s" s="7">
         <v>35</v>
       </c>
-      <c r="D23" s="16"/>
-    </row>
-    <row r="24" ht="13.55" customHeight="1">
-      <c r="A24" t="s" s="8">
+    </row>
+    <row r="26" ht="13.55" customHeight="1">
+      <c r="A26" t="s" s="6">
         <v>36</v>
       </c>
-      <c r="B24" s="9"/>
-      <c r="C24" t="s" s="8">
+      <c r="B26" t="s" s="6">
         <v>37</v>
       </c>
-      <c r="D24" s="9"/>
-    </row>
-    <row r="25" ht="13.55" customHeight="1">
-      <c r="A25" t="s" s="15">
+    </row>
+    <row r="27" ht="13.55" customHeight="1">
+      <c r="A27" t="s" s="7">
         <v>38</v>
       </c>
-      <c r="B25" s="16"/>
-      <c r="C25" t="s" s="15">
+      <c r="B27" t="s" s="7">
         <v>39</v>
       </c>
-      <c r="D25" s="16"/>
-    </row>
-    <row r="26" ht="13.55" customHeight="1">
-      <c r="A26" t="s" s="8">
+    </row>
+    <row r="28" ht="13.55" customHeight="1">
+      <c r="A28" t="s" s="6">
         <v>40</v>
       </c>
-      <c r="B26" s="9"/>
-      <c r="C26" t="s" s="8">
+      <c r="B28" t="s" s="6">
         <v>41</v>
       </c>
-      <c r="D26" s="9"/>
-    </row>
-    <row r="27" ht="13.55" customHeight="1">
-      <c r="A27" t="s" s="15">
+    </row>
+    <row r="29" ht="13.55" customHeight="1">
+      <c r="A29" t="s" s="7">
         <v>42</v>
       </c>
-      <c r="B27" s="16"/>
-      <c r="C27" t="s" s="15">
+      <c r="B29" t="s" s="7">
         <v>43</v>
       </c>
-      <c r="D27" s="16"/>
-    </row>
-    <row r="28" ht="13.55" customHeight="1">
-      <c r="A28" t="s" s="8">
+    </row>
+    <row r="30" ht="13.55" customHeight="1">
+      <c r="A30" t="s" s="6">
         <v>44</v>
       </c>
-      <c r="B28" s="9"/>
-      <c r="C28" t="s" s="8">
+      <c r="B30" t="s" s="6">
         <v>45</v>
       </c>
-      <c r="D28" s="9"/>
-    </row>
-    <row r="29" ht="13.55" customHeight="1">
-      <c r="A29" t="s" s="15">
+    </row>
+    <row r="31" ht="13.55" customHeight="1">
+      <c r="A31" t="s" s="7">
         <v>46</v>
       </c>
-      <c r="B29" s="16"/>
-      <c r="C29" t="s" s="15">
+      <c r="B31" t="s" s="7">
         <v>47</v>
       </c>
-      <c r="D29" s="16"/>
-    </row>
-    <row r="30" ht="13.55" customHeight="1">
-      <c r="A30" t="s" s="8">
+    </row>
+    <row r="32" ht="13.55" customHeight="1">
+      <c r="A32" t="s" s="6">
         <v>48</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" t="s" s="8">
+      <c r="B32" t="s" s="6">
         <v>49</v>
       </c>
     </row>
-    <row r="31" ht="14" customHeight="1">
-      <c r="A31" t="s" s="15">
+    <row r="33" ht="14" customHeight="1">
+      <c r="A33" t="s" s="7">
         <v>50</v>
       </c>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" t="s" s="15">
+      <c r="B33" t="s" s="7">
         <v>51</v>
       </c>
     </row>
-    <row r="32" ht="14" customHeight="1">
-      <c r="A32" t="s" s="21">
+    <row r="34" ht="14" customHeight="1">
+      <c r="A34" t="s" s="16">
         <v>52</v>
       </c>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" t="s" s="21">
+      <c r="B34" s="7"/>
+    </row>
+    <row r="35" ht="13.55" customHeight="1">
+      <c r="A35" t="s" s="6">
         <v>53</v>
       </c>
-    </row>
-    <row r="33" ht="13.55" customHeight="1">
-      <c r="A33" t="s" s="8">
+      <c r="B35" t="s" s="6">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" ht="13.55" customHeight="1">
+      <c r="A36" t="s" s="7">
         <v>54</v>
       </c>
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" t="s" s="8">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="34" ht="13.55" customHeight="1">
-      <c r="A34" t="s" s="15">
+      <c r="B36" t="s" s="7">
         <v>55</v>
       </c>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" t="s" s="15">
+    </row>
+    <row r="37" ht="13.55" customHeight="1">
+      <c r="A37" t="s" s="16">
         <v>56</v>
       </c>
-    </row>
-    <row r="35" ht="13.55" customHeight="1">
-      <c r="A35" t="s" s="21">
+      <c r="B37" s="7"/>
+    </row>
+    <row r="38" ht="13.55" customHeight="1">
+      <c r="A38" t="s" s="11">
+        <v>30</v>
+      </c>
+      <c r="B38" s="12"/>
+    </row>
+    <row r="39" ht="13.55" customHeight="1">
+      <c r="A39" t="s" s="13">
         <v>57</v>
       </c>
-      <c r="B35" s="17"/>
-      <c r="C35" s="17"/>
-      <c r="D35" t="s" s="21">
+      <c r="B39" s="15"/>
+    </row>
+    <row r="40" ht="13.55" customHeight="1">
+      <c r="A40" s="17"/>
+      <c r="B40" s="17"/>
+    </row>
+    <row r="41" ht="13.55" customHeight="1">
+      <c r="A41" t="s" s="18">
         <v>58</v>
       </c>
-    </row>
-    <row r="36" ht="13.55" customHeight="1">
-      <c r="A36" t="s" s="8">
-        <v>30</v>
-      </c>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-    </row>
-    <row r="37" ht="13.55" customHeight="1">
-      <c r="A37" t="s" s="15">
+      <c r="B41" s="19"/>
+    </row>
+    <row r="42" ht="13.55" customHeight="1">
+      <c r="A42" t="s" s="20">
         <v>59</v>
       </c>
-      <c r="B37" s="17"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
-    </row>
-    <row r="38" ht="13.55" customHeight="1">
-      <c r="A38" s="22"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="23"/>
-    </row>
-    <row r="39" ht="13.55" customHeight="1">
-      <c r="A39" t="s" s="24">
+      <c r="B42" t="s" s="20">
         <v>60</v>
       </c>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
-    </row>
-    <row r="40" ht="13.55" customHeight="1">
-      <c r="A40" t="s" s="24">
+    </row>
+    <row r="43" ht="13.55" customHeight="1">
+      <c r="A43" t="s" s="21">
         <v>61</v>
       </c>
-      <c r="B40" t="s" s="24">
+      <c r="B43" t="s" s="21">
         <v>62</v>
       </c>
-      <c r="C40" t="s" s="24">
+    </row>
+    <row r="44" ht="13.55" customHeight="1">
+      <c r="A44" t="s" s="20">
         <v>63</v>
       </c>
-      <c r="D40" t="s" s="24">
+      <c r="B44" t="s" s="20">
         <v>64</v>
       </c>
     </row>
-    <row r="41" ht="13.55" customHeight="1">
-      <c r="A41" t="s" s="26">
+    <row r="45" ht="13.55" customHeight="1">
+      <c r="A45" t="s" s="21">
         <v>65</v>
       </c>
-      <c r="B41" t="s" s="26">
+      <c r="B45" t="s" s="7">
         <v>66</v>
       </c>
-      <c r="C41" t="s" s="26">
+    </row>
+    <row r="46" ht="13.55" customHeight="1">
+      <c r="A46" t="s" s="11">
         <v>67</v>
       </c>
-      <c r="D41" t="s" s="15">
+      <c r="B46" s="12"/>
+    </row>
+    <row r="47" ht="13.55" customHeight="1">
+      <c r="A47" t="s" s="13">
         <v>68</v>
       </c>
-    </row>
-    <row r="42" ht="13.55" customHeight="1">
-      <c r="A42" t="s" s="8">
-        <v>69</v>
-      </c>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-    </row>
-    <row r="43" ht="13.55" customHeight="1">
-      <c r="A43" t="s" s="15">
-        <v>70</v>
-      </c>
-      <c r="B43" s="17"/>
-      <c r="C43" s="17"/>
-      <c r="D43" s="17"/>
+      <c r="B47" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="61">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A37:D37"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
Fix some issues due to rebase
</commit_message>
<xml_diff>
--- a/server/templates/analysisRequest/analysisRequest.xlsx
+++ b/server/templates/analysisRequest/analysisRequest.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="73">
   <si>
     <t>Demande d'Analyse Informatisée</t>
   </si>
@@ -107,6 +107,18 @@
   </si>
   <si>
     <t>{d.notesOnCreation}</t>
+  </si>
+  <si>
+    <t>Catégorie de matrice programmée</t>
+  </si>
+  <si>
+    <t>Code catégorie</t>
+  </si>
+  <si>
+    <t>{d.matrixKindLabel}</t>
+  </si>
+  <si>
+    <t>{d.matrixKind}</t>
   </si>
   <si>
     <t>Matrice</t>
@@ -266,7 +278,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -305,18 +317,34 @@
       <diagonal/>
     </border>
     <border>
-      <left>
+      <left style="thick">
         <color indexed="8"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
-      <top style="medium">
-        <color indexed="8"/>
+      <top style="thin">
+        <color indexed="10"/>
       </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -336,6 +364,31 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="8"/>
       </left>
       <right style="thin">
@@ -350,12 +403,30 @@
       <diagonal/>
     </border>
     <border>
-      <left>
+      <left style="thin">
         <color indexed="8"/>
       </left>
-      <right>
-        <color indexed="8"/>
-      </right>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color indexed="8"/>
       </top>
@@ -398,9 +469,7 @@
       <left style="thin">
         <color indexed="8"/>
       </left>
-      <right>
-        <color indexed="8"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="8"/>
       </top>
@@ -410,9 +479,7 @@
       <diagonal/>
     </border>
     <border>
-      <left>
-        <color indexed="8"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="8"/>
       </right>
@@ -421,6 +488,37 @@
       </top>
       <bottom style="thin">
         <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -430,7 +528,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -444,57 +542,90 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -533,7 +664,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1008775</xdr:colOff>
+      <xdr:colOff>1008774</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>709836</xdr:rowOff>
     </xdr:to>
@@ -554,8 +685,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="19049" y="39290"/>
-          <a:ext cx="989727" cy="670547"/>
+          <a:off x="19050" y="39290"/>
+          <a:ext cx="989725" cy="670546"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1628,14 +1759,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="2" width="50" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="3" max="5" width="8.85156" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="61" customHeight="1">
@@ -1643,332 +1775,495 @@
         <v>0</v>
       </c>
       <c r="B1" s="3"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="6"/>
     </row>
     <row r="2" ht="14.55" customHeight="1">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="6">
+      <c r="A3" t="s" s="11">
         <v>1</v>
       </c>
-      <c r="B3" t="s" s="6">
+      <c r="B3" t="s" s="11">
         <v>2</v>
       </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" ht="42" customHeight="1">
-      <c r="A4" t="s" s="7">
+      <c r="A4" t="s" s="13">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="7">
+      <c r="B4" t="s" s="13">
         <v>4</v>
       </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="10"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" t="s" s="6">
+      <c r="A6" t="s" s="11">
         <v>5</v>
       </c>
-      <c r="B6" t="s" s="6">
+      <c r="B6" t="s" s="11">
         <v>6</v>
       </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" t="s" s="7">
+      <c r="A7" t="s" s="13">
         <v>7</v>
       </c>
-      <c r="B7" t="s" s="7">
+      <c r="B7" t="s" s="13">
         <v>8</v>
       </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" t="s" s="6">
+      <c r="A9" t="s" s="11">
         <v>9</v>
       </c>
-      <c r="B9" t="s" s="6">
+      <c r="B9" t="s" s="11">
         <v>10</v>
       </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" t="s" s="9">
+      <c r="A10" t="s" s="16">
         <v>11</v>
       </c>
-      <c r="B10" t="s" s="10">
+      <c r="B10" t="s" s="17">
         <v>12</v>
       </c>
+      <c r="C10" s="12"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="10"/>
     </row>
     <row r="11" ht="13.55" customHeight="1">
-      <c r="A11" t="s" s="11">
+      <c r="A11" t="s" s="18">
         <v>13</v>
       </c>
-      <c r="B11" s="12"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="10"/>
     </row>
     <row r="12" ht="13.55" customHeight="1">
-      <c r="A12" t="s" s="13">
+      <c r="A12" t="s" s="20">
         <v>14</v>
       </c>
-      <c r="B12" s="14"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="10"/>
     </row>
     <row r="13" ht="13.55" customHeight="1">
-      <c r="A13" t="s" s="6">
+      <c r="A13" t="s" s="11">
         <v>15</v>
       </c>
-      <c r="B13" t="s" s="6">
+      <c r="B13" t="s" s="11">
         <v>16</v>
       </c>
+      <c r="C13" s="12"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="10"/>
     </row>
     <row r="14" ht="13.55" customHeight="1">
-      <c r="A14" t="s" s="9">
+      <c r="A14" t="s" s="16">
         <v>17</v>
       </c>
-      <c r="B14" t="s" s="10">
+      <c r="B14" t="s" s="17">
         <v>18</v>
       </c>
+      <c r="C14" s="12"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="10"/>
     </row>
     <row r="15" ht="13.55" customHeight="1">
-      <c r="A15" t="s" s="6">
+      <c r="A15" t="s" s="11">
         <v>19</v>
       </c>
-      <c r="B15" t="s" s="6">
+      <c r="B15" t="s" s="11">
         <v>20</v>
       </c>
+      <c r="C15" s="12"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" ht="13.55" customHeight="1">
-      <c r="A16" t="s" s="9">
+      <c r="A16" t="s" s="16">
         <v>21</v>
       </c>
-      <c r="B16" t="s" s="10">
+      <c r="B16" t="s" s="17">
         <v>22</v>
       </c>
+      <c r="C16" s="12"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="10"/>
     </row>
     <row r="17" ht="13.55" customHeight="1">
-      <c r="A17" t="s" s="6">
+      <c r="A17" t="s" s="11">
         <v>23</v>
       </c>
-      <c r="B17" t="s" s="6">
+      <c r="B17" t="s" s="11">
         <v>24</v>
       </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="10"/>
     </row>
     <row r="18" ht="13.55" customHeight="1">
-      <c r="A18" t="s" s="9">
+      <c r="A18" t="s" s="16">
         <v>25</v>
       </c>
-      <c r="B18" t="s" s="10">
+      <c r="B18" t="s" s="17">
         <v>26</v>
       </c>
+      <c r="C18" s="12"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="10"/>
     </row>
     <row r="19" ht="13.55" customHeight="1">
-      <c r="A19" t="s" s="6">
+      <c r="A19" t="s" s="11">
         <v>2</v>
       </c>
-      <c r="B19" t="s" s="6">
+      <c r="B19" t="s" s="11">
         <v>27</v>
       </c>
+      <c r="C19" s="12"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="10"/>
     </row>
     <row r="20" ht="28" customHeight="1">
-      <c r="A20" t="s" s="9">
+      <c r="A20" t="s" s="16">
         <v>28</v>
       </c>
-      <c r="B20" t="s" s="10">
+      <c r="B20" t="s" s="17">
         <v>29</v>
       </c>
+      <c r="C20" s="12"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="10"/>
     </row>
     <row r="21" ht="13.55" customHeight="1">
-      <c r="A21" t="s" s="11">
+      <c r="A21" t="s" s="18">
         <v>30</v>
       </c>
-      <c r="B21" s="12"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="10"/>
     </row>
     <row r="22" ht="13.55" customHeight="1">
-      <c r="A22" t="s" s="13">
+      <c r="A22" t="s" s="20">
         <v>31</v>
       </c>
-      <c r="B22" s="15"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="10"/>
     </row>
     <row r="23" ht="13.55" customHeight="1">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
+      <c r="A23" s="14"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="10"/>
     </row>
     <row r="24" ht="13.55" customHeight="1">
-      <c r="A24" t="s" s="6">
+      <c r="A24" t="s" s="11">
         <v>32</v>
       </c>
-      <c r="B24" t="s" s="6">
+      <c r="B24" t="s" s="11">
         <v>33</v>
       </c>
+      <c r="C24" s="12"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="10"/>
     </row>
     <row r="25" ht="13.55" customHeight="1">
-      <c r="A25" t="s" s="7">
+      <c r="A25" t="s" s="13">
         <v>34</v>
       </c>
-      <c r="B25" t="s" s="7">
+      <c r="B25" t="s" s="13">
         <v>35</v>
       </c>
+      <c r="C25" s="12"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="10"/>
     </row>
     <row r="26" ht="13.55" customHeight="1">
-      <c r="A26" t="s" s="6">
+      <c r="A26" t="s" s="11">
         <v>36</v>
       </c>
-      <c r="B26" t="s" s="6">
+      <c r="B26" t="s" s="11">
         <v>37</v>
       </c>
+      <c r="C26" s="12"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="10"/>
     </row>
     <row r="27" ht="13.55" customHeight="1">
-      <c r="A27" t="s" s="7">
+      <c r="A27" t="s" s="13">
         <v>38</v>
       </c>
-      <c r="B27" t="s" s="7">
+      <c r="B27" t="s" s="13">
         <v>39</v>
       </c>
+      <c r="C27" s="12"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="10"/>
     </row>
     <row r="28" ht="13.55" customHeight="1">
-      <c r="A28" t="s" s="6">
+      <c r="A28" t="s" s="11">
         <v>40</v>
       </c>
-      <c r="B28" t="s" s="6">
+      <c r="B28" t="s" s="11">
         <v>41</v>
       </c>
+      <c r="C28" s="12"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="10"/>
     </row>
     <row r="29" ht="13.55" customHeight="1">
-      <c r="A29" t="s" s="7">
+      <c r="A29" t="s" s="13">
         <v>42</v>
       </c>
-      <c r="B29" t="s" s="7">
+      <c r="B29" t="s" s="13">
         <v>43</v>
       </c>
+      <c r="C29" s="12"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="10"/>
     </row>
     <row r="30" ht="13.55" customHeight="1">
-      <c r="A30" t="s" s="6">
+      <c r="A30" t="s" s="11">
         <v>44</v>
       </c>
-      <c r="B30" t="s" s="6">
+      <c r="B30" t="s" s="11">
         <v>45</v>
       </c>
+      <c r="C30" s="12"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="10"/>
     </row>
     <row r="31" ht="13.55" customHeight="1">
-      <c r="A31" t="s" s="7">
+      <c r="A31" t="s" s="13">
         <v>46</v>
       </c>
-      <c r="B31" t="s" s="7">
+      <c r="B31" t="s" s="13">
         <v>47</v>
       </c>
+      <c r="C31" s="12"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="10"/>
     </row>
     <row r="32" ht="13.55" customHeight="1">
-      <c r="A32" t="s" s="6">
+      <c r="A32" t="s" s="11">
         <v>48</v>
       </c>
-      <c r="B32" t="s" s="6">
+      <c r="B32" t="s" s="11">
         <v>49</v>
       </c>
-    </row>
-    <row r="33" ht="14" customHeight="1">
-      <c r="A33" t="s" s="7">
+      <c r="C32" s="12"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="10"/>
+    </row>
+    <row r="33" ht="13.55" customHeight="1">
+      <c r="A33" t="s" s="13">
         <v>50</v>
       </c>
-      <c r="B33" t="s" s="7">
+      <c r="B33" t="s" s="13">
         <v>51</v>
       </c>
-    </row>
-    <row r="34" ht="14" customHeight="1">
-      <c r="A34" t="s" s="16">
+      <c r="C33" s="12"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="10"/>
+    </row>
+    <row r="34" ht="13.55" customHeight="1">
+      <c r="A34" t="s" s="11">
         <v>52</v>
       </c>
-      <c r="B34" s="7"/>
-    </row>
-    <row r="35" ht="13.55" customHeight="1">
-      <c r="A35" t="s" s="6">
+      <c r="B34" t="s" s="11">
         <v>53</v>
       </c>
-      <c r="B35" t="s" s="6">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="36" ht="13.55" customHeight="1">
-      <c r="A36" t="s" s="7">
+      <c r="C34" s="12"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="10"/>
+    </row>
+    <row r="35" ht="14" customHeight="1">
+      <c r="A35" t="s" s="13">
         <v>54</v>
       </c>
-      <c r="B36" t="s" s="7">
+      <c r="B35" t="s" s="13">
         <v>55</v>
       </c>
+      <c r="C35" s="12"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="10"/>
+    </row>
+    <row r="36" ht="14" customHeight="1">
+      <c r="A36" t="s" s="23">
+        <v>56</v>
+      </c>
+      <c r="B36" s="13"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="10"/>
     </row>
     <row r="37" ht="13.55" customHeight="1">
-      <c r="A37" t="s" s="16">
-        <v>56</v>
-      </c>
-      <c r="B37" s="7"/>
+      <c r="A37" t="s" s="11">
+        <v>57</v>
+      </c>
+      <c r="B37" t="s" s="11">
+        <v>53</v>
+      </c>
+      <c r="C37" s="12"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="10"/>
     </row>
     <row r="38" ht="13.55" customHeight="1">
-      <c r="A38" t="s" s="11">
+      <c r="A38" t="s" s="13">
+        <v>58</v>
+      </c>
+      <c r="B38" t="s" s="13">
+        <v>59</v>
+      </c>
+      <c r="C38" s="12"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="10"/>
+    </row>
+    <row r="39" ht="13.55" customHeight="1">
+      <c r="A39" t="s" s="23">
+        <v>60</v>
+      </c>
+      <c r="B39" s="13"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="10"/>
+    </row>
+    <row r="40" ht="13.55" customHeight="1">
+      <c r="A40" t="s" s="18">
         <v>30</v>
       </c>
-      <c r="B38" s="12"/>
-    </row>
-    <row r="39" ht="13.55" customHeight="1">
-      <c r="A39" t="s" s="13">
-        <v>57</v>
-      </c>
-      <c r="B39" s="15"/>
-    </row>
-    <row r="40" ht="13.55" customHeight="1">
-      <c r="A40" s="17"/>
-      <c r="B40" s="17"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="10"/>
     </row>
     <row r="41" ht="13.55" customHeight="1">
-      <c r="A41" t="s" s="18">
-        <v>58</v>
-      </c>
-      <c r="B41" s="19"/>
+      <c r="A41" t="s" s="20">
+        <v>61</v>
+      </c>
+      <c r="B41" s="22"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="10"/>
     </row>
     <row r="42" ht="13.55" customHeight="1">
-      <c r="A42" t="s" s="20">
-        <v>59</v>
-      </c>
-      <c r="B42" t="s" s="20">
-        <v>60</v>
-      </c>
+      <c r="A42" s="24"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="10"/>
     </row>
     <row r="43" ht="13.55" customHeight="1">
-      <c r="A43" t="s" s="21">
-        <v>61</v>
-      </c>
-      <c r="B43" t="s" s="21">
+      <c r="A43" t="s" s="26">
         <v>62</v>
       </c>
+      <c r="B43" s="27"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="10"/>
     </row>
     <row r="44" ht="13.55" customHeight="1">
-      <c r="A44" t="s" s="20">
+      <c r="A44" t="s" s="28">
         <v>63</v>
       </c>
-      <c r="B44" t="s" s="20">
+      <c r="B44" t="s" s="28">
         <v>64</v>
       </c>
+      <c r="C44" s="12"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="10"/>
     </row>
     <row r="45" ht="13.55" customHeight="1">
-      <c r="A45" t="s" s="21">
+      <c r="A45" t="s" s="29">
         <v>65</v>
       </c>
-      <c r="B45" t="s" s="7">
+      <c r="B45" t="s" s="29">
         <v>66</v>
       </c>
+      <c r="C45" s="12"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="10"/>
     </row>
     <row r="46" ht="13.55" customHeight="1">
-      <c r="A46" t="s" s="11">
+      <c r="A46" t="s" s="28">
         <v>67</v>
       </c>
-      <c r="B46" s="12"/>
+      <c r="B46" t="s" s="28">
+        <v>68</v>
+      </c>
+      <c r="C46" s="12"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="10"/>
     </row>
     <row r="47" ht="13.55" customHeight="1">
-      <c r="A47" t="s" s="13">
-        <v>68</v>
-      </c>
-      <c r="B47" s="15"/>
+      <c r="A47" t="s" s="29">
+        <v>69</v>
+      </c>
+      <c r="B47" t="s" s="13">
+        <v>70</v>
+      </c>
+      <c r="C47" s="12"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="10"/>
+    </row>
+    <row r="48" ht="13.55" customHeight="1">
+      <c r="A48" t="s" s="18">
+        <v>71</v>
+      </c>
+      <c r="B48" s="19"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="10"/>
+    </row>
+    <row r="49" ht="13.55" customHeight="1">
+      <c r="A49" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="B49" s="22"/>
+      <c r="C49" s="30"/>
+      <c r="D49" s="31"/>
+      <c r="E49" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>